<commit_message>
xlsx file created by code with new properties added
</commit_message>
<xml_diff>
--- a/contact-company.xlsx
+++ b/contact-company.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A189"/>
+  <dimension ref="A1:A188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,1316 +443,1309 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>recent_deal_close_date</t>
+          <t>days_to_close</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>hs_avatar_filemanager_key</t>
+          <t>hs_date_exited_salesqualifiedlead</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>engagements_last_meeting_booked_medium</t>
+          <t>num_notes</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>notes_next_activity_date</t>
+          <t>hs_notes_next_activity_type</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>hs_last_sales_activity_date</t>
+          <t>hs_shared_team_ids</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>hs_all_team_ids</t>
+          <t>ap_preparer</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>hs_notes_next_activity_type</t>
+          <t>hubspot_owner_id</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>hs_user_ids_of_all_notification_unfollowers</t>
+          <t>hs_time_in_marketingqualifiedlead</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>company_industry</t>
+          <t>hs_date_exited_lead</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>hs_object_source_detail_2</t>
+          <t>total_revenue</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>notes_last_contacted</t>
+          <t>churn_date</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>hs_shared_user_ids</t>
+          <t>estimated_annual_revenue</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>hs_source_object_id</t>
+          <t>owneremail</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>hubspot_owner_assigneddate</t>
+          <t>hs_predictivecontactscore_v2</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>latest_funding_date</t>
+          <t>recent_deal_amount</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>latest_funding_amount</t>
+          <t>cb_custcst_promotional_credits</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>zip</t>
+          <t>profitwell_total_spend</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>date_became_a_lead</t>
+          <t>first_conversion_event_name</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>hs_time_in_114184284</t>
+          <t>hs_notes_next_activity</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>hs_sales_email_last_replied</t>
+          <t>closedate</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>profitwell_created_on</t>
+          <t>hs_analytics_last_visit_timestamp</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>profitwell_total_spend</t>
+          <t>hs_createdate</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>warmlytotalactivetime</t>
+          <t>hs_date_entered_lead</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>first_deal_created_date</t>
+          <t>hs_lead_status</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>engagements_last_meeting_booked_campaign</t>
+          <t>country</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>hs_date_entered_marketingqualifiedlead</t>
+          <t>cb_subcst_plan_unit_price</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>segment</t>
+          <t>hs_time_in_other</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>hs_object_source_user_id</t>
+          <t>hs_updated_by_user_id</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>hs_time_in_customer</t>
+          <t>hs_sales_email_last_replied</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>referral_source</t>
+          <t>hs_analytics_num_page_views</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>profitwell_engagement</t>
+          <t>hs_last_sales_activity_type</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>profitwell_status</t>
+          <t>hs_lastmodifieddate</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>closedate</t>
+          <t>hs_merged_object_ids</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>hs_date_exited_marketingqualifiedlead</t>
+          <t>hs_object_source</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>hs_all_owner_ids</t>
+          <t>hs_analytics_last_timestamp</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>hs_date_exited_evangelist</t>
+          <t>latest_funding_amount</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>hs_object_id</t>
+          <t>num_conversion_events</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>hs_was_imported</t>
+          <t>profitwell_engagement</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>hs_predictivecontactscore_v2</t>
+          <t>hs_object_source_detail_3</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>hs_createdate</t>
+          <t>hs_object_source_label</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>hs_date_exited_customer</t>
+          <t>zip</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>days_to_close</t>
+          <t>hidden_seamless_record_id</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>enrich_with_amplemarket</t>
+          <t>hubspotscore</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>hs_created_by_user_id</t>
+          <t>engagements_last_meeting_booked</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>profitwell_churned_on</t>
+          <t>hs_date_entered_other</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>hs_object_source_detail_3</t>
+          <t>profitwell_activated_on</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>hs_date_exited_salesqualifiedlead</t>
+          <t>warmlytotalpagesviewed</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>hs_date_exited_114184284</t>
+          <t>engagements_last_meeting_booked_source</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>hs_date_entered_salesqualifiedlead</t>
+          <t>hs_all_team_ids</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>hs_date_entered_evangelist</t>
+          <t>hs_analytics_last_touch_converting_campaign</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>hs_time_in_marketingqualifiedlead</t>
+          <t>hs_date_entered_114184284</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>sales_engineer</t>
+          <t>hs_time_in_opportunity</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>hs_date_exited_other</t>
+          <t>cb_subcst_plan_quantity</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>hs_analytics_first_timestamp</t>
+          <t>ownername</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>hs_analytics_last_timestamp</t>
+          <t>business_model</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>amplemarket_sender_first_name</t>
+          <t>city</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>engagements_last_meeting_booked</t>
+          <t>hs_date_entered_161312014</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>hs_lastmodifieddate</t>
+          <t>hs_analytics_first_touch_converting_campaign</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>amplemarket_sender_calendar_link</t>
+          <t>hs_notes_last_activity</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>hs_analytics_source_data_1</t>
+          <t>preparer</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>hs_date_exited_opportunity</t>
+          <t>hs_analytics_first_visit_timestamp</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>warmlycreated</t>
+          <t>hs_time_in_lead</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>annualrevenue</t>
+          <t>accounts_payable_systems</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>city</t>
+          <t>profitwell_status</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>hs_unique_creation_key</t>
+          <t>amplemarket_industry</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>hs_analytics_source</t>
+          <t>profitwell_customer_id</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>hs_object_source_detail_1</t>
+          <t>warmlyutmcampaigns</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>hubspot_owner_id</t>
+          <t>profitwell_churned_on</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>hs_all_accessible_team_ids</t>
+          <t>company_industry</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>hs_analytics_num_visits</t>
+          <t>payroll_provider</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>notes_last_updated</t>
+          <t>what_is_your_revenue_management_tech_stack_</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>hs_last_sales_activity_type</t>
+          <t>warmlylink</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>profitwell_activated_on</t>
+          <t>warmlymatchedsegmentslist</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>hs_all_assigned_business_unit_ids</t>
+          <t>hs_date_entered_opportunity</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>state</t>
+          <t>hs_is_enriched</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>hs_date_entered_other</t>
+          <t>hs_was_imported</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>industry</t>
+          <t>notes_last_updated</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>hs_shared_team_ids</t>
+          <t>hs_time_in_subscriber</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>apollo_recommendation_score</t>
+          <t>hs_date_exited_114184284</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>accounts_payable_systems</t>
+          <t>hs_last_sales_activity_date</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>warmlytotalpagesviewed</t>
+          <t>hs_user_ids_of_all_owners</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>hs_analytics_last_touch_converting_campaign</t>
+          <t>warmlymatchedsegments</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>hs_date_exited_subscriber</t>
+          <t>warmlyutmmediums</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>amplemarket_sender_phone_number</t>
+          <t>warmlytotalsessions</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>amplemarket_industry</t>
+          <t>phone</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>estimated_annual_revenue</t>
+          <t>ap_reviewer</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>hs_date_entered_subscriber</t>
+          <t>warmlyutmsources</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>hs_pinned_engagement_id</t>
+          <t>warmlytotalactivetime</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>hs_user_ids_of_all_owners</t>
+          <t>technologies</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>amplemarket_enrichment_date</t>
+          <t>reviewer</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>hs_date_entered_customer</t>
+          <t>hs_date_exited_subscriber</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>hs_updated_by_user_id</t>
+          <t>hs_user_ids_of_all_notification_followers</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>date_became_a_customer</t>
+          <t>hs_date_exited_161312014</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>hs_notes_last_activity</t>
+          <t>hs_created_by_user_id</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>cb_subcst_plan_quantity</t>
+          <t>date_became_a_customer</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>hs_object_source</t>
+          <t>engagements_last_meeting_booked_medium</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>twitterhandle</t>
+          <t>hs_time_in_evangelist</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>first_conversion_event_name</t>
+          <t>hs_date_exited_other</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>hs_latest_meeting_activity</t>
+          <t>linkedinbio</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>churn_date</t>
+          <t>warmlypagesvisited</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>warmlytotalsessions</t>
+          <t>cb_subcst_plan_amount</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>hs_lead_status</t>
+          <t>profitwell_plans</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>reviewer</t>
+          <t>hs_unique_creation_key</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>hs_date_entered_opportunity</t>
+          <t>do_you_work_with_contractors__if_yes__what_software_do_you_use_to_pay_them_</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>hidden_seamless_job_id</t>
+          <t>date_became_a_sqd</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>warmlyutmsources</t>
+          <t>hubspot_team_id</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>hs_date_entered_114184284</t>
+          <t>hs_date_entered_subscriber</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>cb_subcst_plan_amount</t>
+          <t>hs_latest_meeting_activity</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>date_became_a_sqd</t>
+          <t>hs_avatar_filemanager_key</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>first_conversion_date</t>
+          <t>website</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>hs_time_in_other</t>
+          <t>hs_date_entered_salesqualifiedlead</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>hs_time_in_evangelist</t>
+          <t>annualrevenue</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>hs_object_source_label</t>
+          <t>hs_read_only</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>technologies</t>
+          <t>hs_analytics_first_timestamp</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>hubspotscore</t>
+          <t>hs_time_in_salesqualifiedlead</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>incorporation_type</t>
+          <t>referral_source</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>warmlyutmcontents</t>
+          <t>twitterbio</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>hidden_seamless_record_id</t>
+          <t>enrich_with_amplemarket</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>engagements_last_meeting_booked_source</t>
+          <t>incorporation_type</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>warmlyutmcampaigns</t>
+          <t>latest_funding_date</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>hs_is_enriched</t>
+          <t>createdate</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>lifecyclestage</t>
+          <t>company_technologies</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>hs_time_in_salesqualifiedlead</t>
+          <t>hs_shared_user_ids</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>ownername</t>
+          <t>first_conversion_date</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>hs_analytics_num_page_views</t>
+          <t>hs_object_source_id</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>payroll_provider</t>
+          <t>notes_last_contacted</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>hs_notes_next_activity</t>
+          <t>hs_source_object_id</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>createdate</t>
+          <t>warmlycreated</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>country</t>
+          <t>hs_all_assigned_business_unit_ids</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>hs_time_in_161312014</t>
+          <t>date_became_a_lead</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>num_contacted_notes</t>
+          <t>hs_date_exited_customer</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>hs_analytics_first_visit_timestamp</t>
+          <t>hs_analytics_source_data_2</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>hs_analytics_first_touch_converting_campaign</t>
+          <t>apollo_recommendation_score</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>hubspot_team_id</t>
+          <t>amplemarket_sender_first_name</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>hs_user_ids_of_all_notification_followers</t>
+          <t>hs_all_accessible_team_ids</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>cb_subcst_plan_unit_price</t>
+          <t>hs_pipeline</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>what_is_your_revenue_management_tech_stack_</t>
+          <t>profitwell_created_on</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>num_conversion_events</t>
+          <t>hs_date_exited_evangelist</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>do_you_work_with_contractors__if_yes__what_software_do_you_use_to_pay_them_</t>
+          <t>hs_time_in_114184284</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>num_notes</t>
+          <t>hs_object_id</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>profitwell_mrr</t>
+          <t>latest_funding_stage</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>hs_last_sales_activity_timestamp</t>
+          <t>hs_user_ids_of_all_notification_unfollowers</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>associated_partnership</t>
+          <t>first_deal_created_date</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>created_or_updated_by_amplemarket</t>
+          <t>notes_next_activity_date</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>total_revenue</t>
+          <t>amplemarket_enrichment_date</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>hs_object_source_id</t>
+          <t>warmlyutmcontents</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>ap_reviewer</t>
+          <t>associated_partnership</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>profitwell_customer_id</t>
+          <t>lifecyclestage</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>hs_time_in_opportunity</t>
+          <t>hs_time_in_161312014</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>address</t>
+          <t>num_associated_deals</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>business_model</t>
+          <t>num_contacted_notes</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>hs_pipeline</t>
+          <t>hs_date_entered_customer</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>recent_deal_amount</t>
+          <t>address</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>hs_analytics_source_data_2</t>
+          <t>hs_all_owner_ids</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>ap_preparer</t>
+          <t>hs_analytics_num_visits</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>cb_subcst_plan_free_quantity</t>
+          <t>sales_engineer</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>hs_time_in_subscriber</t>
+          <t>hs_object_source_detail_1</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>warmlylastseenat</t>
+          <t>hs_object_source_user_id</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>associated_partnership_id</t>
+          <t>hs_date_entered_marketingqualifiedlead</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>warmlymatchedsegmentslist</t>
+          <t>amplemarket_sender_calendar_link</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>latest_funding_stage</t>
+          <t>industry</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>num_associated_deals</t>
+          <t>hs_date_exited_opportunity</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>owneremail</t>
+          <t>apollo_enriched</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>hs_read_only</t>
+          <t>recent_conversion_date</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>warmlyutmmediums</t>
+          <t>hs_analytics_source</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>hs_date_exited_lead</t>
+          <t>profitwell_mrr</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>website</t>
+          <t>recent_deal_close_date</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>amplemarket_sender_last_name</t>
+          <t>hs_analytics_source_data_1</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>warmlylink</t>
+          <t>hs_date_entered_evangelist</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>cb_totaldues</t>
+          <t>engagements_last_meeting_booked_campaign</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>hs_date_entered_161312014</t>
+          <t>hs_last_sales_activity_timestamp</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>hs_date_exited_161312014</t>
+          <t>hidden_seamless_job_id</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>recent_conversion_date</t>
+          <t>hs_time_in_customer</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>hs_analytics_last_visit_timestamp</t>
+          <t>hs_date_exited_marketingqualifiedlead</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>hs_merged_object_ids</t>
+          <t>twitterhandle</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>warmlymatchedsegments</t>
+          <t>warmlylastseenat</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>phone</t>
+          <t>associated_partnership_id</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>preparer</t>
+          <t>cb_totaldues</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>apollo_enriched</t>
+          <t>hs_object_source_detail_2</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>company_technologies</t>
+          <t>recent_conversion_event_name</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>cb_custcst_promotional_credits</t>
+          <t>segment</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>hs_time_in_lead</t>
+          <t>amplemarket_sender_last_name</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>warmlypagesvisited</t>
+          <t>state</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>linkedinbio</t>
+          <t>hubspot_owner_assigneddate</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>profitwell_plans</t>
+          <t>hs_pinned_engagement_id</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>recent_conversion_event_name</t>
+          <t>created_or_updated_by_amplemarket</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>twitterbio</t>
-        </is>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" t="inlineStr">
-        <is>
-          <t>hs_date_entered_lead</t>
+          <t>cb_subcst_plan_free_quantity</t>
         </is>
       </c>
     </row>

</xml_diff>